<commit_message>
fixed the 3d models. Note: Lighting affected the accuracy heavily
</commit_message>
<xml_diff>
--- a/dataset/test-3d.xlsx
+++ b/dataset/test-3d.xlsx
@@ -458,19 +458,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.05048991059275004</v>
+        <v>0.05048991059275006</v>
       </c>
       <c r="B2" t="n">
-        <v>0.02141124162030781</v>
+        <v>0.02141124162030787</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.007891432998426302</v>
+        <v>-0.007891432998426255</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005280421204413464</v>
+        <v>0.005280421204413395</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.01310534710632975</v>
+        <v>-0.01310534710632977</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -483,16 +483,16 @@
         <v>0.01518474610401492</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.01333476266455948</v>
+        <v>-0.01333476266455951</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.004076463144678654</v>
+        <v>-0.004076463144678642</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.006277800026380477</v>
+        <v>-0.006277800026380519</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.004062481292655287</v>
+        <v>-0.004062481292655275</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -502,19 +502,19 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.03454084987073196</v>
+        <v>0.03454084987073195</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.01793113040106602</v>
+        <v>-0.01793113040106612</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02480625149676782</v>
+        <v>0.02480625149676778</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002688725700541416</v>
+        <v>0.002688725700541479</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01144752399138456</v>
+        <v>0.01144752399138457</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -524,19 +524,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.001812203404312922</v>
+        <v>-0.00181220340431291</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.01985616769800597</v>
+        <v>-0.019856167698006</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.004302728842824258</v>
+        <v>-0.004302728842824254</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.009135876939842984</v>
+        <v>-0.009135876939843005</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.003326601994861858</v>
+        <v>-0.003326601994861846</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -549,16 +549,16 @@
         <v>-0.01295979278375859</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.0174692383343189</v>
+        <v>-0.01746923833431895</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.008166292494718787</v>
+        <v>-0.008166292494718782</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.01850707590713152</v>
+        <v>-0.01850707590713149</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.003475317533950643</v>
+        <v>-0.003475317533950605</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -568,16 +568,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.003088588952635438</v>
+        <v>-0.00308858895263544</v>
       </c>
       <c r="B7" t="n">
-        <v>0.00616812087994794</v>
+        <v>0.006168120879947936</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0001751350730088109</v>
+        <v>-0.0001751350730088259</v>
       </c>
       <c r="D7" t="n">
-        <v>0.001623965470333184</v>
+        <v>0.001623965470333253</v>
       </c>
       <c r="E7" t="n">
         <v>0.01414591085037823</v>
@@ -590,19 +590,19 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.006079258125723391</v>
+        <v>-0.006079258125723405</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02089141285659926</v>
+        <v>0.02089141285659929</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.002968820108132918</v>
+        <v>-0.00296882010813292</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.00350740647104779</v>
+        <v>-0.003507406471047791</v>
       </c>
       <c r="E8" t="n">
-        <v>0.00445365651830773</v>
+        <v>0.004453656518307737</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -612,19 +612,19 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.02273993773556309</v>
+        <v>-0.0227399377355631</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003057112235920435</v>
+        <v>0.003057112235920437</v>
       </c>
       <c r="C9" t="n">
-        <v>0.008277244428848425</v>
+        <v>0.008277244428848411</v>
       </c>
       <c r="D9" t="n">
-        <v>0.002054673129701509</v>
+        <v>0.002054673129701448</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.01217816908334127</v>
+        <v>-0.01217816908334128</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -637,16 +637,16 @@
         <v>-0.01102438761070081</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02731382643089188</v>
+        <v>0.02731382643089193</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.007561592697452567</v>
+        <v>-0.007561592697452552</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.007776177442258234</v>
+        <v>-0.007776177442258193</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01041564497536401</v>
+        <v>0.01041564497536403</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -656,19 +656,19 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.01275725592825917</v>
+        <v>-0.01275725592825915</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.01823229712505196</v>
+        <v>-0.01823229712505195</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.02133259381673654</v>
+        <v>-0.02133259381673655</v>
       </c>
       <c r="D11" t="n">
         <v>0.02486212733873494</v>
       </c>
       <c r="E11" t="n">
-        <v>0.003364046462956659</v>
+        <v>0.003364046462956584</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -678,19 +678,19 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.02975408202654348</v>
+        <v>-0.0297540820265435</v>
       </c>
       <c r="B12" t="n">
-        <v>0.007981882199335058</v>
+        <v>0.007981882199335042</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02339156325036256</v>
+        <v>0.02339156325036255</v>
       </c>
       <c r="D12" t="n">
-        <v>0.008694423942936576</v>
+        <v>0.008694423942936546</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.007678865787252347</v>
+        <v>-0.007678865787252372</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added 1 more picture of myself to demo dataset
</commit_message>
<xml_diff>
--- a/dataset/test-3d.xlsx
+++ b/dataset/test-3d.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,19 +458,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.05048991059275006</v>
+        <v>-0.03842403594624615</v>
       </c>
       <c r="B2" t="n">
-        <v>0.02141124162030787</v>
+        <v>0.01336580053704416</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.007891432998426255</v>
+        <v>-0.02111056220124395</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005280421204413395</v>
+        <v>0.00503848044508</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.01310534710632977</v>
+        <v>-0.008560712252869118</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -480,151 +480,151 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01518474610401492</v>
+        <v>-0.04110429668360206</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.01333476266455951</v>
+        <v>0.05035112084275228</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.004076463144678642</v>
+        <v>-0.01174729989530701</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.006277800026380519</v>
+        <v>0.004176293938481895</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.004062481292655275</v>
+        <v>-0.001450596453483963</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Phạm Thị Hòa</t>
+          <t>Nguyễn Ngọc Lâm</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.03454084987073195</v>
+        <v>-0.02920324986108187</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.01793113040106612</v>
+        <v>0.01246068639759188</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02480625149676778</v>
+        <v>0.01645955398744802</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002688725700541479</v>
+        <v>0.004946250690690694</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01144752399138457</v>
+        <v>0.008666237927310878</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Nguyễn Minh Khôi</t>
+          <t>Phạm Thị Hòa</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-0.00181220340431291</v>
+        <v>-0.02480676646845765</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.019856167698006</v>
+        <v>0.03087050028332895</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.004302728842824254</v>
+        <v>0.02525817687221753</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.009135876939843005</v>
+        <v>-0.02179462479754733</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.003326601994861846</v>
+        <v>-0.003652766469384778</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Trần Thị Thùy Linh</t>
+          <t>Nguyễn Minh Khôi</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.01295979278375859</v>
+        <v>0.3934377193377001</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.01746923833431895</v>
+        <v>-0.0002005818893808036</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.008166292494718782</v>
+        <v>-0.00238421476150934</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.01850707590713149</v>
+        <v>0.0001985690767570844</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.003475317533950605</v>
+        <v>0.0001089655826942301</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Nguyễn Thị Ngọc Thoa</t>
+          <t>Trần Thị Thùy Linh</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.00308858895263544</v>
+        <v>-0.02967628178700396</v>
       </c>
       <c r="B7" t="n">
-        <v>0.006168120879947936</v>
+        <v>-0.01603961925517172</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0001751350730088259</v>
+        <v>0.01802280440629499</v>
       </c>
       <c r="D7" t="n">
-        <v>0.001623965470333253</v>
+        <v>0.008191921894608059</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01414591085037823</v>
+        <v>0.02120467639060371</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Lê Xuân Quý</t>
+          <t>Nguyễn Thị Ngọc Thoa</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-0.006079258125723405</v>
+        <v>-0.04139033625284454</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02089141285659929</v>
+        <v>-0.004370600022166111</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.00296882010813292</v>
+        <v>0.0009907102970992405</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.003507406471047791</v>
+        <v>-0.0006710254545786845</v>
       </c>
       <c r="E8" t="n">
-        <v>0.004453656518307737</v>
+        <v>0.001174806176446212</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Ma Chí Định</t>
+          <t>Lê Xuân Quý</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-0.0227399377355631</v>
+        <v>-0.04189526835967602</v>
       </c>
       <c r="B9" t="n">
-        <v>0.003057112235920437</v>
+        <v>-0.005724881702870478</v>
       </c>
       <c r="C9" t="n">
-        <v>0.008277244428848411</v>
+        <v>-0.01685239313026183</v>
       </c>
       <c r="D9" t="n">
-        <v>0.002054673129701448</v>
+        <v>0.0004961700871757662</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.01217816908334128</v>
+        <v>0.004659207225906152</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -634,65 +634,87 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-0.01102438761070081</v>
+        <v>-0.03287580758557897</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02731382643089193</v>
+        <v>-0.02420556564215289</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.007561592697452552</v>
+        <v>-0.001501964982323434</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.007776177442258193</v>
+        <v>-0.007763312207248805</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01041564497536403</v>
+        <v>-0.002144893170773051</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Trần Đức Phụng</t>
+          <t>Ma Chí Định</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>-0.01275725592825915</v>
+        <v>-0.04584315835868628</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.01823229712505195</v>
+        <v>-0.01030489015215447</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.02133259381673655</v>
+        <v>-0.02235134079560485</v>
       </c>
       <c r="D11" t="n">
-        <v>0.02486212733873494</v>
+        <v>0.00330848918898061</v>
       </c>
       <c r="E11" t="n">
-        <v>0.003364046462956584</v>
+        <v>0.01006939032269512</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Phạm Thị Hương</t>
+          <t>Trần Đức Phụng</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>-0.0297540820265435</v>
+        <v>-0.03096259279511591</v>
       </c>
       <c r="B12" t="n">
-        <v>0.007981882199335042</v>
+        <v>-0.01500062937872642</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02339156325036255</v>
+        <v>0.01810810838872735</v>
       </c>
       <c r="D12" t="n">
-        <v>0.008694423942936546</v>
+        <v>0.02665995140111898</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.007678865787252372</v>
+        <v>-0.01989623417779658</v>
       </c>
       <c r="F12" t="inlineStr">
+        <is>
+          <t>Phạm Thị Hương</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>-0.03725592523940672</v>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.03120134001809426</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.00289157818553679</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.02278716426351822</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.01017808110134885</v>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>Trần Quốc Việt</t>
         </is>

</xml_diff>